<commit_message>
update for output,renew the cluster
</commit_message>
<xml_diff>
--- a/0530processing_data.xlsx
+++ b/0530processing_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Architecture\AAA-Master\25Spring\ISUF\UrbanFood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309606D2-AA61-4E05-9652-00163C4B58E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142FD9CD-EB52-484E-B762-E8AB27035565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="105" windowWidth="19035" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12585" yWindow="690" windowWidth="19035" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="processing_data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="248">
   <si>
     <t>DENOMINAZI</t>
   </si>
@@ -143,9 +143,6 @@
     <t>POINT (778146.251 5056864.278)</t>
   </si>
   <si>
-    <t>Azienda Agricola Valleri Stefano</t>
-  </si>
-  <si>
     <t>POINT (773095.368 5040347.401)</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>POINT (770259.755 5039188.64)</t>
   </si>
   <si>
-    <t>CAM-EVOLUTION SOCIETA' A RESPONSABILITA' LIMITATA</t>
-  </si>
-  <si>
     <t>Seafood</t>
   </si>
   <si>
@@ -221,9 +215,6 @@
     <t>POINT (770559.813 5039205.504)</t>
   </si>
   <si>
-    <t>CASA VINICOLA CANELLA S.P.A.</t>
-  </si>
-  <si>
     <t>Brewery</t>
   </si>
   <si>
@@ -266,15 +257,9 @@
     <t>POINT (757383.504 5007588.98)</t>
   </si>
   <si>
-    <t>Erma S.r.l.</t>
-  </si>
-  <si>
     <t>POINT (746199.745 5033432.136)</t>
   </si>
   <si>
-    <t>Il Giogo Farm</t>
-  </si>
-  <si>
     <t>POINT (782417.553 5049290.5)</t>
   </si>
   <si>
@@ -284,9 +269,6 @@
     <t>POINT (747290.708 5038830.168)</t>
   </si>
   <si>
-    <t>LA DOLCIARIA MESTRINA DAL 1973 S.R.L.</t>
-  </si>
-  <si>
     <t>POINT (753087.168 5042347.126)</t>
   </si>
   <si>
@@ -326,13 +308,7 @@
     <t>POINT (770361.128 5040818.576)</t>
   </si>
   <si>
-    <t>Miele di Sant'Erasmo di Mavaracchio Elio</t>
-  </si>
-  <si>
     <t>POINT (766405.516 5038795.463)</t>
-  </si>
-  <si>
-    <t>Miglio Rosso</t>
   </si>
   <si>
     <t>POINT (785951.361 5052389.362)</t>
@@ -1103,6 +1079,58 @@
 工业建筑物 #178465304
 工业建筑物 #178468640
 建筑物 #178468291</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Erma S.r.l.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAM-EVOLUTION SOCIETA' A RESPONSABILITA' LIMITATA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seafood</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Azienda Agricola Valleri Stefano</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fruits &amp; Vegetables</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CASA VINICOLA CANELLA S.P.A.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brewery</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miele di Sant'Erasmo di Mavaracchio Elio</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miglio Rosso</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LA DOLCIARIA MESTRINA DAL 1973 S.R.L.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pasta&amp;baked goods</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Il Giogo Farm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dairy</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1490,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1515,12 +1543,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1529,10 +1557,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
@@ -1563,10 +1591,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -1580,10 +1608,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1598,10 +1626,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1616,10 +1644,10 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1634,10 +1662,10 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1652,10 +1680,10 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1670,10 +1698,10 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1688,10 +1716,10 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1706,10 +1734,10 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
@@ -1723,10 +1751,10 @@
         <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -1741,10 +1769,10 @@
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1759,801 +1787,801 @@
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C21" t="s">
         <v>47</v>
       </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
       <c r="D21" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
       </c>
       <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C28" t="s">
         <v>61</v>
       </c>
-      <c r="D27" t="s">
-        <v>173</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" t="s">
+        <v>181</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C36" t="s">
         <v>75</v>
       </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" t="s">
-        <v>187</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" t="s">
-        <v>189</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>80</v>
-      </c>
       <c r="D36" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
         <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3</v>
+      <c r="A38" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D38" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D39" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D41" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" t="s">
-        <v>11</v>
+      <c r="A45" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D45" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>99</v>
+      <c r="A46" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="B46" t="s">
         <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D47" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D49" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D51" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D53" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D54" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
         <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D55" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
         <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D56" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B57" t="s">
         <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D57" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D58" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D59" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -2571,12 +2599,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x010100D190F2CBED6CA84BB6216795005A6A98" ma:contentTypeVersion="4" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="c16965fa2d28f7ee2fd628df83a3e23c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2eba5e38-8e94-466a-bcf6-3de9031f9b5f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52143c88fce8c7fb4308be386231fe32" ns3:_="">
     <xsd:import namespace="2eba5e38-8e94-466a-bcf6-3de9031f9b5f"/>
@@ -2720,6 +2742,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2730,13 +2758,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CC6F1E0-269F-4272-A388-F77ADECFFF39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2D0DE9-411D-414D-96AE-778D71B08D27}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C2D0DE9-411D-414D-96AE-778D71B08D27}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CC6F1E0-269F-4272-A388-F77ADECFFF39}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>